<commit_message>
cours 8 - 9
</commit_message>
<xml_diff>
--- a/_cours/évaluations.xlsx
+++ b/_cours/évaluations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivierross/Documents/professionnel/bioecologie/_cours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86656D3C-0B5B-EB45-8293-277A73C9D273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25242371-ABE0-7C4C-B076-F0D0B1B6F213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="1400" windowWidth="17300" windowHeight="12820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="75">
   <si>
     <t>Audet</t>
   </si>
@@ -1113,7 +1113,8 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1209,6 +1210,9 @@
       <c r="H2" t="s">
         <v>73</v>
       </c>
+      <c r="J2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1235,6 +1239,9 @@
       <c r="H3" t="s">
         <v>73</v>
       </c>
+      <c r="J3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1261,6 +1268,9 @@
       <c r="H4" t="s">
         <v>73</v>
       </c>
+      <c r="J4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1284,6 +1294,9 @@
       <c r="G5" t="s">
         <v>74</v>
       </c>
+      <c r="J5" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1310,6 +1323,9 @@
       <c r="H6" t="s">
         <v>73</v>
       </c>
+      <c r="J6" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1333,6 +1349,9 @@
       <c r="G7" t="s">
         <v>73</v>
       </c>
+      <c r="J7" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1359,6 +1378,9 @@
       <c r="H8" t="s">
         <v>73</v>
       </c>
+      <c r="J8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1385,6 +1407,9 @@
       <c r="H9" t="s">
         <v>73</v>
       </c>
+      <c r="J9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -1408,6 +1433,9 @@
       <c r="G10" t="s">
         <v>73</v>
       </c>
+      <c r="J10" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1434,6 +1462,9 @@
       <c r="H11" t="s">
         <v>73</v>
       </c>
+      <c r="J11" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -1460,6 +1491,9 @@
       <c r="H12" t="s">
         <v>73</v>
       </c>
+      <c r="J12" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1486,6 +1520,9 @@
       <c r="H13" t="s">
         <v>73</v>
       </c>
+      <c r="J13" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1512,6 +1549,9 @@
       <c r="H14" t="s">
         <v>73</v>
       </c>
+      <c r="J14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1538,6 +1578,9 @@
       <c r="H15" t="s">
         <v>73</v>
       </c>
+      <c r="J15" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -1564,8 +1607,11 @@
       <c r="H16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1591,7 +1637,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1616,8 +1662,11 @@
       <c r="H18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1642,8 +1691,11 @@
       <c r="H19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1668,8 +1720,11 @@
       <c r="H20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -1694,8 +1749,11 @@
       <c r="H21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -1720,8 +1778,11 @@
       <c r="H22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1746,8 +1807,11 @@
       <c r="H23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>45</v>
       </c>
@@ -1772,8 +1836,11 @@
       <c r="H24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>47</v>
       </c>
@@ -1798,8 +1865,11 @@
       <c r="H25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1824,8 +1894,11 @@
       <c r="H26" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -1850,8 +1923,11 @@
       <c r="H27" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1867,7 +1943,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1876,7 +1952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C31" s="1">
         <f>SUM(C29:C30)</f>
         <v>26</v>

</xml_diff>